<commit_message>
In progress, going to start making larger changes and graphing it out
</commit_message>
<xml_diff>
--- a/finances.xlsx
+++ b/finances.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28122"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59E2C155-C46B-4EE4-BE2E-842A4C664475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6912E5DE-5D9E-4BC4-9026-B08D96D2E721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,6 +28,32 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Expense</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Water Bill</t>
+  </si>
+  <si>
+    <t>Electric Bill</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -61,8 +87,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,12 +424,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>45569</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>45570</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>45571</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>45573</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added expense category and logic for updating labels and amounts dynamically
</commit_message>
<xml_diff>
--- a/finances.xlsx
+++ b/finances.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6912E5DE-5D9E-4BC4-9026-B08D96D2E721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{19B8A1D7-268A-4353-991F-2FA1047D04AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,11 +31,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
   <si>
+    <t>Category</t>
+  </si>
+  <si>
     <t>Expense</t>
   </si>
   <si>
@@ -45,7 +48,13 @@
     <t>Food</t>
   </si>
   <si>
+    <t>Jersey Mike's</t>
+  </si>
+  <si>
     <t>Gas</t>
+  </si>
+  <si>
+    <t>Bill</t>
   </si>
   <si>
     <t>Water Bill</t>
@@ -424,19 +433,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,59 +456,77 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>45569</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>45570</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>45571</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>45572</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>45573</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6">
         <v>80</v>
       </c>
     </row>

</xml_diff>